<commit_message>
se creo la api que extrae los datos de el excel notas credito masiva v2
</commit_message>
<xml_diff>
--- a/public/formatos/plantilla.xlsx
+++ b/public/formatos/plantilla.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programacion\Tablero-Bots\Backend\public\formatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC8764D3-0B6B-426F-AFF4-E9529D46F2CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4C887F-7907-4A4F-A297-8E1E32B4D1AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2DB4A00D-C20C-4205-B3AC-48940AE1FAEC}"/>
   </bookViews>
@@ -666,7 +666,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="G2" sqref="G2:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.375" defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
se agrego la api para descargar el formato de retiro de usuarios masivo
</commit_message>
<xml_diff>
--- a/public/formatos/plantilla.xlsx
+++ b/public/formatos/plantilla.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programacion\Tablero-Bots\Backend\public\formatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4C887F-7907-4A4F-A297-8E1E32B4D1AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FEDA45E3-8C1F-43A4-96F2-699E5A8DA978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2DB4A00D-C20C-4205-B3AC-48940AE1FAEC}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$2:$BR$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$2:$BR$3</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -30,65 +30,58 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
-    </ext>
-    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
-      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>SEDE</t>
   </si>
   <si>
+    <t>IDENTIFICACION</t>
+  </si>
+  <si>
+    <t>NOMBRE COMPLETO</t>
+  </si>
+  <si>
+    <t>CARGO</t>
+  </si>
+  <si>
+    <t>BUZON COMPARTIDO (SI/NO)</t>
+  </si>
+  <si>
+    <t>CUENTA A DELEGAR</t>
+  </si>
+  <si>
     <t>FECHA DE RETIRO</t>
   </si>
   <si>
     <t xml:space="preserve">DIACOR SOACHA ZONA FRANCA </t>
   </si>
   <si>
-    <t>LUZ JESSENIA MARTINEZ CARDENAS</t>
+    <t>MARIO DE JESUS BOLIVAR</t>
   </si>
   <si>
     <t>AUXILIAR ENFERMERIA SALA DE PARTOS</t>
   </si>
   <si>
-    <t>VALERIA SANCHEZ ROJAS</t>
-  </si>
-  <si>
-    <t>AUXILIAR ENFERMERIA HOSPITALIZACION</t>
-  </si>
-  <si>
-    <t>BLANCA LIZETH HERNANDEZ MONTEALEGRE</t>
-  </si>
-  <si>
-    <t>AUXILIAR LABORATORIO</t>
-  </si>
-  <si>
-    <t>NOMBRE COMPLETO</t>
-  </si>
-  <si>
-    <t>CARGO</t>
-  </si>
-  <si>
-    <t>CUENTA A DELEGAR</t>
-  </si>
-  <si>
-    <t>BUZON COMPARTIDO (SI/NO)</t>
-  </si>
-  <si>
-    <t>IDENTIFICACION</t>
+    <t>si</t>
+  </si>
+  <si>
+    <t>cuenta@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,6 +112,14 @@
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -159,10 +160,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -188,8 +190,10 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="14">
@@ -663,20 +667,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95EE2686-5C37-46EE-89EA-E25AD5BFF75F}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G4"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.375" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="32.125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="32.140625" style="4" customWidth="1"/>
     <col min="2" max="2" width="14" style="3" customWidth="1"/>
-    <col min="3" max="3" width="38.25" style="1" customWidth="1"/>
-    <col min="4" max="6" width="25.625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.375" style="2"/>
-    <col min="8" max="16384" width="11.375" style="1"/>
+    <col min="3" max="3" width="38.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="34.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="25.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="2"/>
+    <col min="8" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25.5">
@@ -684,106 +689,81 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="5" customFormat="1" ht="15">
+      <c r="A2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="7">
+        <v>100522522</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="9" t="s">
+      <c r="F2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="5" customFormat="1">
-      <c r="A2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="7">
-        <v>1012414400</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
       <c r="G2" s="8">
         <v>45828</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="7">
-        <v>1014479338</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="8">
-        <v>45831</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="7">
-        <v>1024528582</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="8">
-        <v>45821</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A2:BR5" xr:uid="{95EE2686-5C37-46EE-89EA-E25AD5BFF75F}"/>
-  <conditionalFormatting sqref="B6:B1048576 B1:B4">
+  <autoFilter ref="A2:BR3" xr:uid="{95EE2686-5C37-46EE-89EA-E25AD5BFF75F}"/>
+  <conditionalFormatting sqref="B4:B1048576 B1:B2">
     <cfRule type="duplicateValues" dxfId="13" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B4">
-    <cfRule type="duplicateValues" dxfId="12" priority="23"/>
+  <conditionalFormatting sqref="B4:B1048576">
+    <cfRule type="duplicateValues" dxfId="12" priority="77"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6:B1048576">
-    <cfRule type="duplicateValues" dxfId="11" priority="77"/>
+  <conditionalFormatting sqref="B4:B1048576 B1">
+    <cfRule type="duplicateValues" dxfId="11" priority="81"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="82"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="83"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="84"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="85"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="86"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="87"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="88"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="89"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="90"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="91"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6:B1048576 B1">
-    <cfRule type="duplicateValues" dxfId="10" priority="81"/>
-    <cfRule type="duplicateValues" dxfId="9" priority="82"/>
-    <cfRule type="duplicateValues" dxfId="8" priority="83"/>
-    <cfRule type="duplicateValues" dxfId="7" priority="84"/>
-    <cfRule type="duplicateValues" dxfId="6" priority="85"/>
-    <cfRule type="duplicateValues" dxfId="5" priority="86"/>
-    <cfRule type="duplicateValues" dxfId="4" priority="87"/>
-    <cfRule type="duplicateValues" dxfId="3" priority="88"/>
-    <cfRule type="duplicateValues" dxfId="2" priority="89"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="90"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="91"/>
+  <conditionalFormatting sqref="B2">
+    <cfRule type="duplicateValues" dxfId="0" priority="93"/>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{BBAC1038-9A61-4C08-BABA-E94249F57D2F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{e0aea30c-d719-4efa-9135-ced50768b536}" enabled="1" method="Standard" siteId="{c9ef7bf6-bbe0-4c50-b2e9-ea58d635ca46}" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>